<commit_message>
Added statistics about whole country
</commit_message>
<xml_diff>
--- a/data/countys.xlsx
+++ b/data/countys.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl Rapur\OneDrive - Tartu Ülikool\Töölaud\LTAT.02.002_Sissejuhatus_andmeteadusesse\IDS2020Project\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -129,10 +124,10 @@
     <t>UNIVERSAAL</t>
   </si>
   <si>
-    <t>TOYOTA 11.2</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN 15.2</t>
+    <t>TOYOTA 11.3</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN 15.3</t>
   </si>
   <si>
     <t>VOLKSWAGEN 13.3</t>
@@ -153,25 +148,25 @@
     <t>VOLKSWAGEN 10.8</t>
   </si>
   <si>
-    <t>VOLKSWAGEN 13.4</t>
+    <t>VOLKSWAGEN 13.5</t>
   </si>
   <si>
     <t>VOLKSWAGEN 11.2</t>
   </si>
   <si>
-    <t>VOLKSWAGEN 15.9</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN 19.0</t>
+    <t>VOLKSWAGEN 16.0</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN 19.1</t>
   </si>
   <si>
     <t>VOLKSWAGEN 18.8</t>
   </si>
   <si>
-    <t>VOLKSWAGEN 11.0</t>
-  </si>
-  <si>
-    <t>VOLKSWAGEN 12.8</t>
+    <t>VOLKSWAGEN 11.1</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN 12.7</t>
   </si>
   <si>
     <t>VOLKSWAGEN 9.8</t>
@@ -189,7 +184,7 @@
     <t>TOYOTA 11.1</t>
   </si>
   <si>
-    <t>AUDI 8.1</t>
+    <t>AUDI 8.2</t>
   </si>
   <si>
     <t>AUDI 10.3</t>
@@ -210,7 +205,7 @@
     <t>AUDI 8.8</t>
   </si>
   <si>
-    <t>AUDI 9.8</t>
+    <t>AUDI 9.9</t>
   </si>
   <si>
     <t>TOYOTA 8.7</t>
@@ -222,7 +217,7 @@
     <t>BMW 6.7</t>
   </si>
   <si>
-    <t>FORD 7.8</t>
+    <t>FORD 7.9</t>
   </si>
   <si>
     <t>BMW 6.8</t>
@@ -243,7 +238,7 @@
     <t>AUDI 7.9</t>
   </si>
   <si>
-    <t>AUDI 6.3</t>
+    <t>AUDI 6.4</t>
   </si>
   <si>
     <t>TOYOTA 8.8</t>
@@ -258,13 +253,13 @@
     <t>FORD 8.7</t>
   </si>
   <si>
-    <t>VOLVO 6.9</t>
+    <t>VOLVO 7.0</t>
   </si>
   <si>
     <t>BMW 6.5</t>
   </si>
   <si>
-    <t>OCTAVIA 2.6</t>
+    <t>OCTAVIA 2.7</t>
   </si>
   <si>
     <t>PASSAT VARIANT 3.3</t>
@@ -309,42 +304,42 @@
     <t>OCTAVIA 2.5</t>
   </si>
   <si>
+    <t>PASSAT 2.9</t>
+  </si>
+  <si>
+    <t>CR-V 2.4</t>
+  </si>
+  <si>
+    <t>PASSAT 2.3</t>
+  </si>
+  <si>
+    <t>PASSAT 2.7</t>
+  </si>
+  <si>
+    <t>PASSAT 3.6</t>
+  </si>
+  <si>
+    <t>PASSAT VARIANT 2.2</t>
+  </si>
+  <si>
+    <t>PASSAT 2.6</t>
+  </si>
+  <si>
+    <t>A6 AVANT 2.2</t>
+  </si>
+  <si>
+    <t>PASSAT 3.1</t>
+  </si>
+  <si>
+    <t>PASSAT 3.2</t>
+  </si>
+  <si>
+    <t>COROLLA 2.2</t>
+  </si>
+  <si>
     <t>AVENSIS 2.4</t>
   </si>
   <si>
-    <t>PASSAT 2.9</t>
-  </si>
-  <si>
-    <t>CR-V 2.4</t>
-  </si>
-  <si>
-    <t>PASSAT 2.3</t>
-  </si>
-  <si>
-    <t>PASSAT 2.7</t>
-  </si>
-  <si>
-    <t>PASSAT 3.6</t>
-  </si>
-  <si>
-    <t>PASSAT VARIANT 2.2</t>
-  </si>
-  <si>
-    <t>PASSAT 2.6</t>
-  </si>
-  <si>
-    <t>A6 AVANT 2.2</t>
-  </si>
-  <si>
-    <t>PASSAT 3.1</t>
-  </si>
-  <si>
-    <t>PASSAT 3.2</t>
-  </si>
-  <si>
-    <t>COROLLA 2.2</t>
-  </si>
-  <si>
     <t>COROLLA 2.3</t>
   </si>
   <si>
@@ -354,7 +349,7 @@
     <t>AVENSIS 2.3</t>
   </si>
   <si>
-    <t>A6 AVANT 2.9</t>
+    <t>A6 AVANT 3.0</t>
   </si>
   <si>
     <t>OCTAVIA 2.3</t>
@@ -384,8 +379,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,18 +397,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -443,29 +432,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -512,7 +489,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,10 +521,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,7 +555,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -755,22 +730,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,66 +793,66 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:19">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3">
-        <v>280727</v>
-      </c>
-      <c r="D2" s="3">
-        <v>9.56</v>
-      </c>
-      <c r="E2" s="3">
-        <v>54.11</v>
-      </c>
-      <c r="F2" s="3">
-        <v>58.44</v>
-      </c>
-      <c r="G2" s="3">
-        <v>40.869999999999997</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="C2">
+        <v>279746</v>
+      </c>
+      <c r="D2">
+        <v>9.59</v>
+      </c>
+      <c r="E2">
+        <v>54.14</v>
+      </c>
+      <c r="F2">
+        <v>58.65</v>
+      </c>
+      <c r="G2">
+        <v>41.02</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3">
-        <v>109.8849269931288</v>
-      </c>
-      <c r="L2" s="3">
-        <v>160.8148506257842</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1568.7883103513379</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="K2">
+        <v>110.0208156684995</v>
+      </c>
+      <c r="L2">
+        <v>161.5009010229659</v>
+      </c>
+      <c r="M2">
+        <v>1568.812726544794</v>
+      </c>
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" t="s">
         <v>66</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" t="s">
         <v>81</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" t="s">
         <v>89</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -893,22 +860,22 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>70275</v>
+        <v>70128</v>
       </c>
       <c r="D3">
-        <v>6.95</v>
+        <v>6.96</v>
       </c>
       <c r="E3">
-        <v>44.49</v>
+        <v>44.48</v>
       </c>
       <c r="F3">
-        <v>50.49</v>
+        <v>50.6</v>
       </c>
       <c r="G3">
-        <v>48.86</v>
+        <v>48.96</v>
       </c>
       <c r="H3">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
@@ -917,13 +884,13 @@
         <v>35</v>
       </c>
       <c r="K3">
-        <v>106.2803941657772</v>
+        <v>106.3701003878621</v>
       </c>
       <c r="L3">
-        <v>164.79496686651939</v>
+        <v>165.2610510076937</v>
       </c>
       <c r="M3">
-        <v>1570.1715972963359</v>
+        <v>1570.380076431668</v>
       </c>
       <c r="N3" t="s">
         <v>37</v>
@@ -938,72 +905,72 @@
         <v>82</v>
       </c>
       <c r="R3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:19">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3">
-        <v>50557</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4">
+        <v>50532</v>
+      </c>
+      <c r="D4">
         <v>10.82</v>
       </c>
-      <c r="E4" s="3">
-        <v>39.11</v>
-      </c>
-      <c r="F4" s="3">
-        <v>48.23</v>
-      </c>
-      <c r="G4" s="3">
-        <v>51.57</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="E4">
+        <v>39.09</v>
+      </c>
+      <c r="F4">
+        <v>48.26</v>
+      </c>
+      <c r="G4">
+        <v>51.6</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="3">
-        <v>102.8087544751469</v>
-      </c>
-      <c r="L4" s="3">
-        <v>170.89127715889589</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1573.435805130842</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="K4">
+        <v>102.8325536293834</v>
+      </c>
+      <c r="L4">
+        <v>171.015630457562</v>
+      </c>
+      <c r="M4">
+        <v>1573.507322092931</v>
+      </c>
+      <c r="N4" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" t="s">
         <v>83</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="R4" t="s">
+        <v>97</v>
+      </c>
+      <c r="S4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1011,22 +978,22 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>40973</v>
+        <v>40906</v>
       </c>
       <c r="D5">
-        <v>7.87</v>
+        <v>7.88</v>
       </c>
       <c r="E5">
-        <v>43.36</v>
+        <v>43.35</v>
       </c>
       <c r="F5">
-        <v>51.84</v>
+        <v>51.92</v>
       </c>
       <c r="G5">
-        <v>47.63</v>
+        <v>47.7</v>
       </c>
       <c r="H5">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="I5" t="s">
         <v>34</v>
@@ -1035,13 +1002,13 @@
         <v>35</v>
       </c>
       <c r="K5">
-        <v>104.1971176140385</v>
+        <v>104.264887791522</v>
       </c>
       <c r="L5">
-        <v>166.82125890736339</v>
+        <v>167.2008892623324</v>
       </c>
       <c r="M5">
-        <v>1550.2879945329851</v>
+        <v>1550.47812056911</v>
       </c>
       <c r="N5" t="s">
         <v>39</v>
@@ -1062,66 +1029,66 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:19">
+      <c r="A6" s="1">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3">
-        <v>29192</v>
-      </c>
-      <c r="D6" s="3">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="E6" s="3">
-        <v>38.270000000000003</v>
-      </c>
-      <c r="F6" s="3">
-        <v>50.22</v>
-      </c>
-      <c r="G6" s="3">
-        <v>49.42</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="C6">
+        <v>29156</v>
+      </c>
+      <c r="D6">
+        <v>8.73</v>
+      </c>
+      <c r="E6">
+        <v>38.22</v>
+      </c>
+      <c r="F6">
+        <v>50.28</v>
+      </c>
+      <c r="G6">
+        <v>49.49</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="3">
-        <v>101.2792271855303</v>
-      </c>
-      <c r="L6" s="3">
-        <v>166.6256606432778</v>
-      </c>
-      <c r="M6" s="3">
-        <v>1542.583858591395</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="K6">
+        <v>101.346865139251</v>
+      </c>
+      <c r="L6">
+        <v>166.9281428067167</v>
+      </c>
+      <c r="M6">
+        <v>1542.881602414597</v>
+      </c>
+      <c r="N6" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" t="s">
         <v>70</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" t="s">
         <v>85</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>102</v>
+      <c r="R6" t="s">
+        <v>98</v>
+      </c>
+      <c r="S6" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1129,22 +1096,22 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>24223</v>
+        <v>24163</v>
       </c>
       <c r="D7">
-        <v>7.99</v>
+        <v>8.01</v>
       </c>
       <c r="E7">
-        <v>39.47</v>
+        <v>39.4</v>
       </c>
       <c r="F7">
-        <v>50.7</v>
+        <v>50.82</v>
       </c>
       <c r="G7">
-        <v>48.8</v>
+        <v>48.93</v>
       </c>
       <c r="H7">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>34</v>
@@ -1153,13 +1120,13 @@
         <v>35</v>
       </c>
       <c r="K7">
-        <v>100.87449531437071</v>
+        <v>100.9873318710426</v>
       </c>
       <c r="L7">
-        <v>164.29610756385071</v>
+        <v>164.8934007024462</v>
       </c>
       <c r="M7">
-        <v>1535.333814969244</v>
+        <v>1535.656085750941</v>
       </c>
       <c r="N7" t="s">
         <v>40</v>
@@ -1174,72 +1141,72 @@
         <v>86</v>
       </c>
       <c r="R7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:19">
+      <c r="A8" s="1">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="3">
-        <v>19212</v>
-      </c>
-      <c r="D8" s="3">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="E8" s="3">
-        <v>33.53</v>
-      </c>
-      <c r="F8" s="3">
-        <v>42.45</v>
-      </c>
-      <c r="G8" s="3">
-        <v>57.14</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="C8">
+        <v>19173</v>
+      </c>
+      <c r="D8">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="E8">
+        <v>33.45</v>
+      </c>
+      <c r="F8">
+        <v>42.54</v>
+      </c>
+      <c r="G8">
+        <v>57.26</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="3">
-        <v>99.87674370185303</v>
-      </c>
-      <c r="L8" s="3">
-        <v>165.4419168687798</v>
-      </c>
-      <c r="M8" s="3">
-        <v>1538.6821257547369</v>
-      </c>
-      <c r="N8" s="3" t="s">
+      <c r="K8">
+        <v>99.98195378918273</v>
+      </c>
+      <c r="L8">
+        <v>165.9833025675449</v>
+      </c>
+      <c r="M8">
+        <v>1539.144265373181</v>
+      </c>
+      <c r="N8" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" t="s">
         <v>57</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" t="s">
         <v>72</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="S8" s="3" t="s">
+      <c r="R8" t="s">
+        <v>100</v>
+      </c>
+      <c r="S8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -1247,22 +1214,22 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>18255</v>
+        <v>18233</v>
       </c>
       <c r="D9">
-        <v>8.44</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="E9">
-        <v>42.97</v>
+        <v>42.94</v>
       </c>
       <c r="F9">
-        <v>50.31</v>
+        <v>50.38</v>
       </c>
       <c r="G9">
-        <v>49.42</v>
+        <v>49.48</v>
       </c>
       <c r="H9">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="I9" t="s">
         <v>34</v>
@@ -1271,13 +1238,13 @@
         <v>35</v>
       </c>
       <c r="K9">
-        <v>102.8584278279924</v>
+        <v>102.9172160368563</v>
       </c>
       <c r="L9">
-        <v>165.45480472154011</v>
+        <v>165.7305189652436</v>
       </c>
       <c r="M9">
-        <v>1551.253190906601</v>
+        <v>1551.473591838973</v>
       </c>
       <c r="N9" t="s">
         <v>42</v>
@@ -1298,66 +1265,66 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:19">
+      <c r="A10" s="1">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3">
-        <v>18046</v>
-      </c>
-      <c r="D10" s="3">
-        <v>5.62</v>
-      </c>
-      <c r="E10" s="3">
-        <v>40.11</v>
-      </c>
-      <c r="F10" s="3">
-        <v>58.01</v>
-      </c>
-      <c r="G10" s="3">
-        <v>41.58</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="C10">
+        <v>17992</v>
+      </c>
+      <c r="D10">
+        <v>5.64</v>
+      </c>
+      <c r="E10">
+        <v>40.02</v>
+      </c>
+      <c r="F10">
+        <v>58.18</v>
+      </c>
+      <c r="G10">
+        <v>41.7</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="3">
-        <v>100.8285880527541</v>
-      </c>
-      <c r="L10" s="3">
-        <v>166.520876056107</v>
-      </c>
-      <c r="M10" s="3">
-        <v>1523.387675939266</v>
-      </c>
-      <c r="N10" s="3" t="s">
+      <c r="K10">
+        <v>100.9664684304135</v>
+      </c>
+      <c r="L10">
+        <v>167.2617615555739</v>
+      </c>
+      <c r="M10">
+        <v>1523.773454868831</v>
+      </c>
+      <c r="N10" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" t="s">
         <v>59</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" t="s">
         <v>74</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q10" t="s">
         <v>89</v>
       </c>
-      <c r="R10" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="S10" s="3" t="s">
+      <c r="R10" t="s">
+        <v>101</v>
+      </c>
+      <c r="S10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1365,22 +1332,22 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>15461</v>
+        <v>15431</v>
       </c>
       <c r="D11">
-        <v>8.7200000000000006</v>
+        <v>8.74</v>
       </c>
       <c r="E11">
-        <v>37.26</v>
+        <v>37.19</v>
       </c>
       <c r="F11">
-        <v>49.25</v>
+        <v>49.34</v>
       </c>
       <c r="G11">
-        <v>50.42</v>
+        <v>50.52</v>
       </c>
       <c r="H11">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
         <v>34</v>
@@ -1389,13 +1356,13 @@
         <v>35</v>
       </c>
       <c r="K11">
-        <v>101.7334907185822</v>
+        <v>101.8223381504763</v>
       </c>
       <c r="L11">
-        <v>166.8556081214272</v>
+        <v>167.3504349545275</v>
       </c>
       <c r="M11">
-        <v>1539.461419054395</v>
+        <v>1539.740651934418</v>
       </c>
       <c r="N11" t="s">
         <v>44</v>
@@ -1410,72 +1377,72 @@
         <v>90</v>
       </c>
       <c r="R11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:19">
+      <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3">
-        <v>14867</v>
-      </c>
-      <c r="D12" s="3">
-        <v>26.41</v>
-      </c>
-      <c r="E12" s="3">
-        <v>48.6</v>
-      </c>
-      <c r="F12" s="3">
-        <v>51.85</v>
-      </c>
-      <c r="G12" s="3">
-        <v>47.97</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="C12">
+        <v>14859</v>
+      </c>
+      <c r="D12">
+        <v>26.43</v>
+      </c>
+      <c r="E12">
+        <v>48.58</v>
+      </c>
+      <c r="F12">
+        <v>51.88</v>
+      </c>
+      <c r="G12">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="3">
-        <v>111.5234277258357</v>
-      </c>
-      <c r="L12" s="3">
-        <v>179.18945334697119</v>
-      </c>
-      <c r="M12" s="3">
-        <v>1589.4069415483959</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="K12">
+        <v>111.5515041389057</v>
+      </c>
+      <c r="L12">
+        <v>179.352519622341</v>
+      </c>
+      <c r="M12">
+        <v>1589.568207820176</v>
+      </c>
+      <c r="N12" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" t="s">
         <v>61</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" t="s">
         <v>76</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="Q12" t="s">
         <v>91</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="S12" s="3" t="s">
+      <c r="R12" t="s">
+        <v>103</v>
+      </c>
+      <c r="S12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1483,22 +1450,22 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>14454</v>
+        <v>14429</v>
       </c>
       <c r="D13">
-        <v>7.86</v>
+        <v>7.87</v>
       </c>
       <c r="E13">
-        <v>35.590000000000003</v>
+        <v>35.49</v>
       </c>
       <c r="F13">
-        <v>46.02</v>
+        <v>46.1</v>
       </c>
       <c r="G13">
-        <v>53.58</v>
+        <v>53.68</v>
       </c>
       <c r="H13">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
@@ -1507,13 +1474,13 @@
         <v>35</v>
       </c>
       <c r="K13">
-        <v>100.25772104607719</v>
+        <v>100.347709473976</v>
       </c>
       <c r="L13">
-        <v>166.9791041577368</v>
+        <v>167.4276351133555</v>
       </c>
       <c r="M13">
-        <v>1541.765116922651</v>
+        <v>1542.155866657426</v>
       </c>
       <c r="N13" t="s">
         <v>46</v>
@@ -1528,72 +1495,72 @@
         <v>92</v>
       </c>
       <c r="R13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:19">
+      <c r="A14" s="1">
         <v>7</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3">
-        <v>14305</v>
-      </c>
-      <c r="D14" s="3">
-        <v>9.0500000000000007</v>
-      </c>
-      <c r="E14" s="3">
-        <v>32.75</v>
-      </c>
-      <c r="F14" s="3">
-        <v>45.7</v>
-      </c>
-      <c r="G14" s="3">
-        <v>53.62</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.38</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="C14">
+        <v>14250</v>
+      </c>
+      <c r="D14">
+        <v>9.08</v>
+      </c>
+      <c r="E14">
+        <v>32.74</v>
+      </c>
+      <c r="F14">
+        <v>45.87</v>
+      </c>
+      <c r="G14">
+        <v>53.82</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" t="s">
         <v>35</v>
       </c>
-      <c r="K14" s="3">
-        <v>99.211541419084242</v>
-      </c>
-      <c r="L14" s="3">
-        <v>167.17361829254281</v>
-      </c>
-      <c r="M14" s="3">
-        <v>1537.96798322265</v>
-      </c>
-      <c r="N14" s="3" t="s">
+      <c r="K14">
+        <v>99.3272350877193</v>
+      </c>
+      <c r="L14">
+        <v>168.2368177613321</v>
+      </c>
+      <c r="M14">
+        <v>1538.297263157895</v>
+      </c>
+      <c r="N14" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" t="s">
         <v>63</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" t="s">
         <v>67</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" t="s">
         <v>93</v>
       </c>
-      <c r="R14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" s="3" t="s">
+      <c r="R14" t="s">
+        <v>100</v>
+      </c>
+      <c r="S14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -1601,22 +1568,22 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>14186</v>
+        <v>14158</v>
       </c>
       <c r="D15">
-        <v>9.4</v>
+        <v>9.42</v>
       </c>
       <c r="E15">
-        <v>33.03</v>
+        <v>32.93</v>
       </c>
       <c r="F15">
-        <v>43.61</v>
+        <v>43.7</v>
       </c>
       <c r="G15">
-        <v>56.03</v>
+        <v>56.14</v>
       </c>
       <c r="H15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>34</v>
@@ -1625,13 +1592,13 @@
         <v>35</v>
       </c>
       <c r="K15">
-        <v>100.26699562949391</v>
+        <v>100.375731035457</v>
       </c>
       <c r="L15">
-        <v>168.15286908077991</v>
+        <v>168.6791103163071</v>
       </c>
       <c r="M15">
-        <v>1549.174185817003</v>
+        <v>1549.649950557988</v>
       </c>
       <c r="N15" t="s">
         <v>48</v>
@@ -1646,72 +1613,72 @@
         <v>94</v>
       </c>
       <c r="R15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:19">
+      <c r="A16" s="1">
         <v>9</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3">
-        <v>11154</v>
-      </c>
-      <c r="D16" s="3">
-        <v>7.26</v>
-      </c>
-      <c r="E16" s="3">
-        <v>42.74</v>
-      </c>
-      <c r="F16" s="3">
-        <v>55.86</v>
-      </c>
-      <c r="G16" s="3">
-        <v>43.22</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="C16">
+        <v>11132</v>
+      </c>
+      <c r="D16">
+        <v>7.28</v>
+      </c>
+      <c r="E16">
+        <v>42.68</v>
+      </c>
+      <c r="F16">
+        <v>55.97</v>
+      </c>
+      <c r="G16">
+        <v>43.31</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="3">
-        <v>101.12301416532191</v>
-      </c>
-      <c r="L16" s="3">
-        <v>162.41643383286771</v>
-      </c>
-      <c r="M16" s="3">
-        <v>1524.597722790031</v>
-      </c>
-      <c r="N16" s="3" t="s">
+      <c r="K16">
+        <v>101.2242274523895</v>
+      </c>
+      <c r="L16">
+        <v>162.8714977075904</v>
+      </c>
+      <c r="M16">
+        <v>1524.757815307222</v>
+      </c>
+      <c r="N16" t="s">
         <v>49</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" t="s">
         <v>64</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" t="s">
         <v>79</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" t="s">
         <v>95</v>
       </c>
-      <c r="R16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="S16" s="3" t="s">
+      <c r="R16" t="s">
+        <v>106</v>
+      </c>
+      <c r="S16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1719,22 +1686,22 @@
         <v>33</v>
       </c>
       <c r="C17">
-        <v>5635</v>
+        <v>5626</v>
       </c>
       <c r="D17">
-        <v>5.91</v>
+        <v>5.92</v>
       </c>
       <c r="E17">
-        <v>40.369999999999997</v>
+        <v>40.31</v>
       </c>
       <c r="F17">
-        <v>54.04</v>
+        <v>54.12</v>
       </c>
       <c r="G17">
-        <v>45.77</v>
+        <v>45.84</v>
       </c>
       <c r="H17">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>34</v>
@@ -1743,13 +1710,13 @@
         <v>35</v>
       </c>
       <c r="K17">
-        <v>101.1832298136646</v>
+        <v>101.2597760398152</v>
       </c>
       <c r="L17">
-        <v>168.96771632707069</v>
+        <v>169.3710875331565</v>
       </c>
       <c r="M17">
-        <v>1540.292990239574</v>
+        <v>1540.671347316033</v>
       </c>
       <c r="N17" t="s">
         <v>50</v>
@@ -1761,10 +1728,10 @@
         <v>80</v>
       </c>
       <c r="Q17" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="R17" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="S17" t="s">
         <v>119</v>
@@ -1772,6 +1739,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>